<commit_message>
se actualizan los documentos de modelo logico y arquitectura tecnica con las nuevas fuentes de bd
</commit_message>
<xml_diff>
--- a/Analisis/BD_complemento.xlsx
+++ b/Analisis/BD_complemento.xlsx
@@ -518,9 +518,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -620,7 +618,7 @@
   <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I38" sqref="I38"/>
+      <selection sqref="A1:B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -704,12 +702,12 @@
   <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+      <selection sqref="A1:G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.28515625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="16.28515625" style="1" customWidth="1"/>
     <col min="2" max="2" width="14.7109375" style="1" customWidth="1"/>
     <col min="3" max="4" width="11.42578125" style="1"/>
     <col min="5" max="5" width="28.28515625" style="1" customWidth="1"/>
@@ -877,7 +875,7 @@
   <dimension ref="A1:K15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+      <selection sqref="A1:K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1122,7 +1120,7 @@
   <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="C15" sqref="A1:C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1224,7 +1222,7 @@
   <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+      <selection sqref="A1:E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1362,7 +1360,7 @@
   <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+      <selection sqref="A1:B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1446,7 +1444,7 @@
   <dimension ref="A1:K15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+      <selection sqref="A1:K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1692,7 +1690,7 @@
   <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H39" sqref="H39"/>
+      <selection sqref="A1:H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1883,7 +1881,7 @@
   <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F32" sqref="F32"/>
+      <selection sqref="A1:F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2039,7 +2037,7 @@
   <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I25" sqref="I25"/>
+      <selection sqref="A1:C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>